<commit_message>
fix the academic-pdf-report bug
</commit_message>
<xml_diff>
--- a/tasks/finalpool/academic-pdf-report/initial_workspace/paper_initial.xlsx
+++ b/tasks/finalpool/academic-pdf-report/initial_workspace/paper_initial.xlsx
@@ -38,7 +38,7 @@
     <t>Affiliation</t>
   </si>
   <si>
-    <t>Google Personal Website</t>
+    <t>Personal Website</t>
   </si>
   <si>
     <t>Strategy Coopetition Explains the Emergence and Transience of In-Context Learning</t>
@@ -72,7 +72,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +82,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -558,148 +551,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1057,7 +1050,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Update academic-pdf-report task files
</commit_message>
<xml_diff>
--- a/tasks/finalpool/academic-pdf-report/initial_workspace/paper_initial.xlsx
+++ b/tasks/finalpool/academic-pdf-report/initial_workspace/paper_initial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19160" windowHeight="10760"/>
+    <workbookView windowWidth="30240" windowHeight="13400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Title</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Affiliation</t>
   </si>
   <si>
-    <t>Personal Website</t>
+    <t>Google Scholar Profile</t>
   </si>
   <si>
     <t>Strategy Coopetition Explains the Emergence and Transience of In-Context Learning</t>
@@ -58,25 +58,22 @@
   <si>
     <t>Learning Smooth and Expressive Interatomic Potentials for Physical Property Prediction</t>
   </si>
-  <si>
-    <t>Multi-agent Architecture Search via Agentic Supernet</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -84,7 +81,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -92,7 +89,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -100,14 +97,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -115,7 +112,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -123,7 +120,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -131,7 +128,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -139,7 +136,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -147,14 +144,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -162,7 +159,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +167,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -178,14 +175,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -193,42 +190,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -551,19 +548,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -703,55 +700,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1047,13 +1044,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -1099,11 +1096,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>